<commit_message>
documentation changes preparing for openpyxl migration
</commit_message>
<xml_diff>
--- a/acrylic/testdata.xlsx
+++ b/acrylic/testdata.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="96" windowWidth="28752" windowHeight="12588"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="28755" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
   <si>
     <t>james</t>
   </si>
@@ -85,16 +85,25 @@
   </si>
   <si>
     <t>ペトロ</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,7 +249,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -275,7 +283,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -451,22 +458,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.109375" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" customWidth="1"/>
     <col min="3" max="3" width="40" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -486,7 +493,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -506,7 +513,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -526,7 +533,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -546,7 +553,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -566,7 +573,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -586,7 +593,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -606,7 +613,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -626,7 +633,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -646,7 +653,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -666,7 +673,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -686,7 +693,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -706,7 +713,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -736,24 +743,74 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added a second sheet to testdata.xlsx
</commit_message>
<xml_diff>
--- a/acrylic/testdata.xlsx
+++ b/acrylic/testdata.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="96" windowWidth="28752" windowHeight="12588"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="28755" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
   <si>
     <t>james</t>
   </si>
@@ -85,16 +85,25 @@
   </si>
   <si>
     <t>ペトロ</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,7 +249,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -275,7 +283,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -451,22 +458,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.109375" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" customWidth="1"/>
     <col min="3" max="3" width="40" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -486,7 +493,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -506,7 +513,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -526,7 +533,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -546,7 +553,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -566,7 +573,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -586,7 +593,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -606,7 +613,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -626,7 +633,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -646,7 +653,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -666,7 +673,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -686,7 +693,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -706,7 +713,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -736,24 +743,74 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>